<commit_message>
why Im work at 5am
</commit_message>
<xml_diff>
--- a/data/新增 Microsoft Excel 工作表.xlsx
+++ b/data/新增 Microsoft Excel 工作表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Desktop\大學修課\基物實\phys_exp6\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCF28FE-2FB3-4E9E-83DE-8B0B3EDCEDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3D5586-6D00-42FD-A991-3547A4C502B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>d1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>dave(cm)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -113,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -121,13 +133,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -408,15 +510,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -427,41 +533,41 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>86</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>120</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>57.6</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2.3599999999999999E-2</v>
       </c>
-      <c r="H2">
-        <f>C$1*G2*C$6/C$5/F2/E2</f>
+      <c r="I2">
+        <f>C$1*H2*C$6/C$5/G2/F2</f>
         <v>1.045515102668946</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -469,21 +575,21 @@
         <f>86-5.2</f>
         <v>80.8</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>60</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>56.4</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="H3">
-        <f>C$1*G3*C$6/C$5/F3/E3</f>
+      <c r="I3">
+        <f>C$1*H3*C$6/C$5/G3/F3</f>
         <v>1.2034923215720432</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -495,21 +601,21 @@
         <f>B4/100</f>
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>180</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>60.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="H4">
-        <f>C$1*G4*C$6/C$5/F4/E4</f>
+      <c r="I4">
+        <f>C$1*H4*C$6/C$5/G4/F4</f>
         <v>0.8773012566225038</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -522,7 +628,7 @@
         <v>5.4628840494007555E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -534,7 +640,7 @@
         <v>334560.00000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -545,48 +651,48 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
         <v>80.900000000000006</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>70</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>38</v>
       </c>
-      <c r="G9">
-        <f>L9-J9</f>
+      <c r="H9">
+        <f>N9-L9</f>
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="H9">
-        <f>C$1*G9*C$6/C$12/F9/E9</f>
+      <c r="I9">
+        <f>C$1*H9*C$6/C$12/G9/F9</f>
         <v>0.83295466732641366</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>7.0499999999999998E-3</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>1.3849999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -594,28 +700,28 @@
         <f>86-5.2</f>
         <v>80.8</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>60</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>39</v>
       </c>
-      <c r="G10">
-        <f>L10-J10</f>
+      <c r="H10">
+        <f>N10-L10</f>
         <v>6.5099999999999993E-3</v>
       </c>
-      <c r="H10">
-        <f>C$1*G10*C$6/C$12/F10/E10</f>
+      <c r="I10">
+        <f>C$1*H10*C$6/C$12/G10/F10</f>
         <v>0.90648207593165986</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>7.0499999999999998E-3</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>1.3559999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -627,28 +733,28 @@
         <f>B11/100</f>
         <v>8.0849999999999991E-2</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>70</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>43</v>
       </c>
-      <c r="G11">
-        <f>L11-J11</f>
+      <c r="H11">
+        <f>N11-L11</f>
         <v>7.4500000000000009E-3</v>
       </c>
-      <c r="H11">
-        <f>C$1*G11*C$6/C$12/F11/E11</f>
+      <c r="I11">
+        <f>C$1*H11*C$6/C$12/G11/F11</f>
         <v>0.80646192311938347</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>7.0499999999999998E-3</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -661,7 +767,7 @@
         <v>5.133929846138776E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -673,144 +779,314 @@
         <v>334560.00000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>0.5</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="5">
+        <f>0.001/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="J15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>80.900000000000006</v>
       </c>
-      <c r="E16" s="1">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3">
         <v>70</v>
       </c>
-      <c r="F16">
+      <c r="G16" s="2">
         <v>66</v>
       </c>
-      <c r="G16">
-        <f>(L16-J16)*1.05</f>
+      <c r="H16" s="2">
+        <f>(N16-L16)*1.05</f>
         <v>1.8637500000000001E-2</v>
       </c>
-      <c r="H16">
-        <f>C$1*G16*C$6/C$12/F16/E16</f>
+      <c r="I16" s="2">
+        <f>C$1*H16*C$6/C$12/G16/F16</f>
         <v>1.314436985889593</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
+        <f>G16/$C$15/$C$20*F16*$D$19</f>
+        <v>1.0125284479978396E-2</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2">
         <v>6.7499999999999999E-3</v>
       </c>
-      <c r="L16">
+      <c r="M16" s="2"/>
+      <c r="N16" s="8">
         <v>2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <f>86-5.2</f>
         <v>80.8</v>
       </c>
-      <c r="E17">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <v>60</v>
       </c>
-      <c r="F17">
+      <c r="G17" s="2">
         <v>66</v>
       </c>
-      <c r="G17">
-        <f>L17-J17</f>
+      <c r="H17" s="2">
+        <f>N17-L17</f>
         <v>1.6149999999999998E-2</v>
       </c>
-      <c r="H17">
-        <f>C$1*G17*C$6/C$12/F17/E17</f>
+      <c r="I17" s="2">
+        <f>C$1*H17*C$6/C$12/G17/F17</f>
         <v>1.3288361390996506</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="2">
+        <f>G17/$C$15/$C$20*F17*$D$19</f>
+        <v>8.6788152685529103E-3</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="L17">
+      <c r="M17" s="2"/>
+      <c r="N17" s="8">
         <v>8.6249999999999993E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <f>AVERAGE(B16:B17)/10</f>
         <v>8.0849999999999991</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <f>B18/100</f>
         <v>8.0849999999999991E-2</v>
       </c>
-      <c r="E18">
+      <c r="D18" s="2">
+        <f>0.001/SQRT(12)</f>
+        <v>2.886751345948129E-4</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
         <v>120</v>
       </c>
-      <c r="F18">
+      <c r="G18" s="2">
         <v>67</v>
       </c>
-      <c r="G18">
-        <f>L18-J18</f>
+      <c r="H18" s="2">
+        <f>N18-L18</f>
         <v>3.2750000000000001E-2</v>
       </c>
-      <c r="H18">
-        <f>C$1*G18*C$6/C$12/F18/E18</f>
+      <c r="I18" s="2">
+        <f>C$1*H18*C$6/C$12/G18/F18</f>
         <v>1.3272396445006684</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
+        <f>G18/$C$15/$C$20*F18*$D$19</f>
+        <v>1.7620624939183184E-2</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="L18">
+      <c r="M18" s="2"/>
+      <c r="N18" s="8">
         <v>0.10285</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <f>B18^2*PI()/4</f>
         <v>51.339298461387756</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <f>C18^2*PI()/4</f>
         <v>5.133929846138776E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="D19" s="2">
+        <f>B18*PI()/2*D18</f>
+        <v>3.6661419649584122E-3</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>80</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <f>B20*4.182/0.001</f>
         <v>334560.00000000006</v>
       </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <f>1/SQRT(12)</f>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G20" s="2">
+        <f>1/SQRT(12)</f>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H20" s="2">
+        <f>0.00005/SQRT(12)</f>
+        <v>1.4433756729740646E-5</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <f>SQRT(SUMSQ(J16/G16*G20,J16/F16*F20,J16/$C$15*$D$15,J16*$D$19/$C$19))</f>
+        <v>7.2543195553011076E-3</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" s="7"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <f t="shared" ref="F21:G22" si="0">1/SQRT(12)</f>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" ref="H21:H22" si="1">0.00005/SQRT(12)</f>
+        <v>1.4433756729740646E-5</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <f>SQRT(SUMSQ(J17/G17*G21,J17/F17*F21,J17/$C$15*$D$15,J17*$D$19/$C$19))</f>
+        <v>6.218025386856567E-3</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4433756729740646E-5</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
+        <f>SQRT(SUMSQ(J18/G18*G22,J18/F18*F22,J18/$C$15*$D$15,J18*$D$19/$C$19))</f>
+        <v>1.2624255323892076E-2</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" s="7"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>